<commit_message>
feature: allow to specify blank_values (by default equals to None and "")
</commit_message>
<xml_diff>
--- a/tests/data/dynamic/counter5.DR_MY_CUSTOM.xlsx
+++ b/tests/data/dynamic/counter5.DR_MY_CUSTOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="62">
   <si>
     <t xml:space="preserve">Report_Name</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total_Item_Investigations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zero</t>
   </si>
   <si>
     <t xml:space="preserve">Total_Item_Requests</t>
@@ -462,7 +465,7 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1135,8 +1138,8 @@
       <c r="K16" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="L16" s="11" t="n">
-        <v>0</v>
+      <c r="L16" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="M16" s="11" t="n">
         <v>0</v>
@@ -1201,7 +1204,7 @@
         <v>42</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K17" s="10" t="n">
         <v>75</v>
@@ -1272,7 +1275,7 @@
         <v>42</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K18" s="10" t="n">
         <v>16</v>
@@ -1343,7 +1346,7 @@
         <v>42</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K19" s="10" t="n">
         <v>2</v>
@@ -1414,7 +1417,7 @@
         <v>42</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K20" s="10" t="n">
         <v>1</v>
@@ -1476,7 +1479,7 @@
         <v>39</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>41</v>
@@ -1547,7 +1550,7 @@
         <v>47</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>41</v>
@@ -1612,13 +1615,13 @@
         <v>45</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>41</v>
@@ -1683,13 +1686,13 @@
         <v>51</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>41</v>
@@ -1760,7 +1763,7 @@
         <v>53</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>41</v>
@@ -1831,7 +1834,7 @@
         <v>39</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>41</v>
@@ -1902,7 +1905,7 @@
         <v>47</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>41</v>
@@ -1967,13 +1970,13 @@
         <v>45</v>
       </c>
       <c r="E28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>41</v>
@@ -2038,13 +2041,13 @@
         <v>51</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>41</v>
@@ -2115,7 +2118,7 @@
         <v>39</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>41</v>
@@ -2124,7 +2127,7 @@
         <v>42</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K30" s="10" t="n">
         <v>8</v>
@@ -2186,7 +2189,7 @@
         <v>47</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>41</v>
@@ -2195,7 +2198,7 @@
         <v>42</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K31" s="10" t="n">
         <v>19</v>
@@ -2251,13 +2254,13 @@
         <v>45</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>41</v>
@@ -2266,7 +2269,7 @@
         <v>42</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K32" s="10" t="n">
         <v>309</v>
@@ -2322,13 +2325,13 @@
         <v>51</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>41</v>
@@ -2337,7 +2340,7 @@
         <v>42</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K33" s="10" t="n">
         <v>3</v>

</xml_diff>